<commit_message>
modificacion orden y nombre de columnas
</commit_message>
<xml_diff>
--- a/Agrupación de datos y decisiones.xlsx
+++ b/Agrupación de datos y decisiones.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Adalab\PROYECTO\Modulo 3\project-da-promo-k-modulo-3-team-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F743BE2C-08D6-425A-8152-E202F5ACC205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAF8E42-B2B3-4430-B3BB-04D375AEC7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{C7B29ED3-7BA0-4949-A03C-A8C9623641E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{C7B29ED3-7BA0-4949-A03C-A8C9623641E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Consideraciones generales" sheetId="7" r:id="rId1"/>
     <sheet name="Tabla principal" sheetId="2" r:id="rId2"/>
     <sheet name="Experiencia profesional" sheetId="10" r:id="rId3"/>
-    <sheet name="Implicación con la empresa" sheetId="8" r:id="rId4"/>
-    <sheet name="Condiciones laborales" sheetId="9" r:id="rId5"/>
-    <sheet name="Satisfacción" sheetId="5" r:id="rId6"/>
-    <sheet name="Datos personales" sheetId="1" r:id="rId7"/>
-    <sheet name="Salario" sheetId="3" r:id="rId8"/>
-    <sheet name="departamentos" sheetId="6" r:id="rId9"/>
+    <sheet name="Condiciones laborales" sheetId="9" r:id="rId4"/>
+    <sheet name="Satisfacción" sheetId="5" r:id="rId5"/>
+    <sheet name="Datos personales" sheetId="1" r:id="rId6"/>
+    <sheet name="Salario" sheetId="3" r:id="rId7"/>
+    <sheet name="departamentos" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="210">
   <si>
     <t>Campo</t>
   </si>
@@ -156,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 'educationfield'</t>
-  </si>
-  <si>
-    <t>: 'Life Sciences', 'Technical Degree', 'Medical' 'Other' 'Marketing', 'Human Resources.'</t>
   </si>
   <si>
     <t xml:space="preserve"> 'employeecount'</t>
@@ -479,56 +475,6 @@
 * No hay ningún dato no nulo
 * Valorara prescindir de él
 </t>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Los salarios de los empleados están duplicados por meses y años y horas. Creo que algunos campos corresponden a los datos del empleado y otros a la categoría o puesto de trabajo. Estudiar separar esta última tabla</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Agrupar los datos que se refieren a la satisfacción del empleado?? O será la tabla principal??</t>
-    </r>
   </si>
   <si>
     <r>
@@ -553,31 +499,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Localizar las moscas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Agrupar los datos que tengan que ver con el puesto y su jerarquía</t>
     </r>
   </si>
   <si>
@@ -715,9 +636,6 @@
     </r>
   </si>
   <si>
-    <t>Cambiar 'divorced' 'Marreid' por los correctos</t>
-  </si>
-  <si>
     <t>department</t>
   </si>
   <si>
@@ -725,9 +643,6 @@
   </si>
   <si>
     <t>no data</t>
-  </si>
-  <si>
-    <t>Se crea esta columna con los datos complementados entre department y roledepartment</t>
   </si>
   <si>
     <t>* Se han quitado los símbolos
@@ -736,6 +651,36 @@
   </si>
   <si>
     <t>* Consideramos los valores negativos como errores al introductirlos. Los cambiamos por positivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Se cambian todos los caracteres a minúsculas
+* Se utiliza para rellenar los datos y luego se elimina
+</t>
+  </si>
+  <si>
+    <t>* Se cambian todos los caracteres a minúsculas para facilitar su estudio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+* Se cambian todos los caracteres a minúsculas para facilitar su estudio
+* Se ha utilizado para rellenar department y luego se ha eliminado</t>
+  </si>
+  <si>
+    <t>Es el id de la tabla principal y lo heredarán todas las demás tablas</t>
+  </si>
+  <si>
+    <t>Una vez que tengamos todos los id de empleados correctos, tenemos que resetear index, para que tengamos un autoincrement a employee_number que pasar a SQL</t>
+  </si>
+  <si>
+    <t>* Consultado con el cliente: Los datos nulos, son Full time</t>
+  </si>
+  <si>
+    <t>* Se redondea a 2 decimales
+* Consultado con el cliente la full-time son 8 horas</t>
+  </si>
+  <si>
+    <t>* Se redondea a 2 decimales
+* Consultado con el salario diario del trabajador se calculó (hourlyrate * 2 )+(hourlyrate * 2*30% )</t>
   </si>
   <si>
     <r>
@@ -751,45 +696,160 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>* Falta intentar rellenar los datos</t>
+      <t>* Falta intentar rellenar los datos. Rellenados con salay
+* Consultado con el cliente
+monthlyincome	salary	employeenumber
+1316	84083.0	10090.0	1317
+1359	87667.0	10520.0	1360
+1464	94083.0	11290.0	1465
+Hemos modificado  monthlyincome basándonos en salary/12</t>
     </r>
-  </si>
-  <si>
-    <t>* Se cambia a tipo float</t>
-  </si>
-  <si>
-    <t>Se cambian los números decimales por enteros y cambiar float por int</t>
-  </si>
-  <si>
-    <t>Se redondea a 2 decimales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Se cambian todos los caracteres a minúsculas
-* Se utiliza para rellenar los datos y luego se elimina
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
-  </si>
-  <si>
-    <t>* Se cambian todos los caracteres a minúsculas para facilitar su estudio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-* Se cambian todos los caracteres a minúsculas para facilitar su estudio
-* Se ha utilizado para rellenar department y luego se ha eliminado</t>
-  </si>
-  <si>
-    <t>Es el id de la tabla principal y lo heredarán todas las demás tablas</t>
+    </r>
+  </si>
+  <si>
+    <t>Dailyrate</t>
+  </si>
+  <si>
+    <t>Ratio = dr/1,3/2</t>
+  </si>
+  <si>
+    <t>Tablas salariales</t>
+  </si>
+  <si>
+    <t>joblevel+jobrole</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>inc subida</t>
+  </si>
+  <si>
+    <t>Pelao</t>
+  </si>
+  <si>
+    <t>1+research scientist</t>
+  </si>
+  <si>
+    <t>pelao</t>
+  </si>
+  <si>
+    <t>mesrate</t>
+  </si>
+  <si>
+    <t>añorate</t>
+  </si>
+  <si>
+    <t>diarate</t>
+  </si>
+  <si>
+    <t>coste</t>
+  </si>
+  <si>
+    <t>saldiario</t>
+  </si>
+  <si>
+    <t>salmes</t>
+  </si>
+  <si>
+    <t>salaño</t>
+  </si>
+  <si>
+    <t>Salario convenio</t>
+  </si>
+  <si>
+    <t>subida salarial</t>
+  </si>
+  <si>
+    <t>total anual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                       Salario del empleado </t>
+  </si>
+  <si>
+    <t>Full time horas =</t>
+  </si>
+  <si>
+    <t>Part time horas=</t>
+  </si>
+  <si>
+    <t>1+research scientist---6 año</t>
+  </si>
+  <si>
+    <t>1+research scientist----1 años</t>
+  </si>
+  <si>
+    <t>Ver cálculos en elena_limpieza ---- elena proyecto</t>
+  </si>
+  <si>
+    <t>??? Al cliente si hay un convenio. Si todo el mundo empieza cobrando igual y en qué se basan las subidas salariales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">???? </t>
+  </si>
+  <si>
+    <t>worklifebalance no podermos  cambiar de float a int hasta que no quitemos los nulos</t>
   </si>
   <si>
     <t xml:space="preserve">* Demasiados valores nulos
 * Se pueden rellar con  'yearssincelastpromotion'
-* Pero son tan pocos datos y algunos herróneos que consideramos borrarlo. Ya que este dato lo podemos conseguir haciendo una diferencia </t>
+</t>
+  </si>
+  <si>
+    <t>Life Sciences', 'Technical Degree', 'Medical' 'Other' 'Marketing', 'Human Resources.', others</t>
+  </si>
+  <si>
+    <t>Se cambian los números decimales por enteros y cambiar float por int
+Intentar por la media o mediana. O técnica avanzada de imputación y describe para ver si se van de madre</t>
+  </si>
+  <si>
+    <t>Se crea esta columna con los datos complementados entre department y roledepartment. Pueden ser manager generales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Se cambia a tipo float
+* Consideramos que los nan son not rated
+</t>
+  </si>
+  <si>
+    <t>Cambiar 'divorced' 'Marreid' por los correctos
+Consultado con el cliente. Cambiar los nulos por unknown</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Los dejamos como nulos y solo estudiamos los no nulos, si nos hiciera falta
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Hay que cambiarlo a float, que es como está el resto de esta categoría</t>
+    </r>
+  </si>
+  <si>
+    <t>* Se cambian todos los caracteres a minúsculas para facilitar su estudio
+* Cambiar los no data por others</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -907,8 +967,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,6 +997,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -995,9 +1068,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1007,26 +1077,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1065,12 +1123,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1080,20 +1132,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1188,14 +1231,77 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1512,64 +1618,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB25C6F-76B8-4E16-A67C-AFB4F956F9F5}">
-  <dimension ref="A2:B12"/>
+  <dimension ref="A2:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
-        <v>144</v>
+      <c r="B5" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
-        <v>145</v>
+      <c r="B6" s="17" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
-        <v>146</v>
+      <c r="B7" s="71" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
-        <v>138</v>
-      </c>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
-        <v>139</v>
-      </c>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>140</v>
+      <c r="A11" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>141</v>
+      <c r="A12" s="16"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1578,7 +1684,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,117 +1738,117 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="C2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="49">
+        <v>1</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="59">
-        <v>1</v>
-      </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="56" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>41</v>
-      </c>
       <c r="B3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="13" t="s">
-        <v>46</v>
+      <c r="D3" s="15"/>
+      <c r="E3" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="K3" s="38" t="s">
-        <v>45</v>
+        <v>168</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="65" t="s">
+      <c r="A4" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="68" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="65" t="s">
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="55" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="41">
+        <v>200</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="46">
-        <v>200</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="K5" s="38" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="26"/>
+      <c r="B12" s="21"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
+      <c r="B13" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1752,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB41178A-9FD0-4F8D-B8D0-1936090A3AB7}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,230 +1913,153 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="43"/>
+      <c r="F2" s="36">
+        <v>549</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="K2" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="46">
-        <v>549</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="41" t="s">
+    </row>
+    <row r="3" spans="1:11" s="50" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="46">
+      <c r="E3" s="49"/>
+      <c r="F3" s="42">
         <v>1643</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="38" t="s">
-        <v>179</v>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="65" t="s">
+      <c r="A4" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="55"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C5" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="65"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="65" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="66" t="s">
+    </row>
+    <row r="6" spans="1:11" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="65" t="s">
-        <v>129</v>
-      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="51"/>
+    </row>
+    <row r="7" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="51"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6415F3-C871-4B5B-97CE-06ADD5F19215}">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="6"/>
-    <col min="4" max="4" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" style="7" customWidth="1"/>
-    <col min="6" max="7" width="11.5546875" style="6"/>
-    <col min="8" max="8" width="18.77734375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" style="3"/>
-    <col min="10" max="10" width="39.21875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="45.88671875" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="61"/>
-    </row>
-    <row r="3" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="61"/>
-    </row>
-    <row r="4" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="61"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B08A03-6272-4CED-8CF6-AED2D39E93E8}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2083,141 +2112,137 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="11"/>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="46">
+      <c r="F2" s="36">
         <v>696</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="14"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="15" t="s">
-        <v>88</v>
+      <c r="K2" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="F3" s="41">
+        <v>351</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="46">
-        <v>351</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="41">
+        <v>801</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="41"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="11">
-        <v>801</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="24" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="38" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="46">
-        <v>114</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>116</v>
+      <c r="E6" s="58"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" s="55" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2226,12 +2251,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893C116-BEF8-4F70-993B-C062F9A68F4A}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2283,75 +2308,132 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:11" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="C2" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="61" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="65" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="56"/>
+      <c r="E4" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="66" t="s">
+      <c r="E5" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="36">
+        <v>114</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="65" t="s">
-        <v>96</v>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="51"/>
+    </row>
+    <row r="10" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="72" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2359,12 +2441,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313F02A3-3B67-4E29-B894-592374DB9B55}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2417,238 +2499,216 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="C4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="90" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="41">
+        <v>774</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" s="91"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="K4" s="92" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" s="48" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="66" t="s">
+      <c r="D5" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="41">
+        <v>675</v>
+      </c>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="38" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="E7" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="42">
+        <v>938</v>
+      </c>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="47" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="56"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="68"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="65" t="s">
-        <v>170</v>
-      </c>
-      <c r="K3" s="65" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="62" t="s">
+      <c r="D9" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="46">
-        <v>774</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="63">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="K6" s="61" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="46">
-        <v>675</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="48" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="52">
-        <v>938</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55" t="s">
+      <c r="E9" s="49"/>
+      <c r="F9" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="56" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="57" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="65" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="60" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="52" t="s">
+      <c r="K9" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="56" t="s">
-        <v>137</v>
-      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2656,12 +2716,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9D7E35-C134-47BF-8225-BED5DA93994C}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,13 +2731,14 @@
     <col min="3" max="3" width="11.5546875" style="6"/>
     <col min="4" max="4" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="7" customWidth="1"/>
-    <col min="6" max="8" width="11.5546875" style="6"/>
+    <col min="6" max="6" width="16.44140625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="11.5546875" style="6"/>
     <col min="9" max="9" width="11.5546875" style="3"/>
     <col min="10" max="10" width="30.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="75.77734375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2712,58 +2773,58 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+    <row r="2" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="41"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="46"/>
+    </row>
+    <row r="3" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="86">
+        <v>1267</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="56"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="72">
-        <v>1267</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="K3" s="38" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>4</v>
@@ -2771,177 +2832,506 @@
       <c r="D4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="267.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="C5" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="41">
+        <v>489</v>
+      </c>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="51" t="s">
+    </row>
+    <row r="6" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+    </row>
+    <row r="7" spans="1:12" s="23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="53"/>
-      <c r="F5" s="51">
+      <c r="E8" s="67"/>
+      <c r="F8" s="42">
         <v>489</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="65" t="s">
-        <v>171</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="62" t="s">
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="58"/>
+      <c r="F9" s="56">
+        <v>0</v>
+      </c>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" s="55" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-    </row>
-    <row r="7" spans="1:11" s="28" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="62" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="21"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="84" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="82" t="s">
+        <v>190</v>
+      </c>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="82" t="s">
+        <v>175</v>
+      </c>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="75" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="79" t="s">
+        <v>182</v>
+      </c>
+      <c r="J21" s="85" t="s">
+        <v>193</v>
+      </c>
+      <c r="K21" s="85"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="76" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="75" t="s">
+        <v>183</v>
+      </c>
+      <c r="F22" s="75" t="s">
+        <v>184</v>
+      </c>
+      <c r="G22" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="78" t="s">
+        <v>188</v>
+      </c>
+      <c r="I22" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="78"/>
+      <c r="I23" s="79"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="5">
         <v>8</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="52">
-        <v>489</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="66">
-        <v>0</v>
-      </c>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" s="65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="28" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="K10" s="61" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="26"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="79"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>626</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="75">
+        <v>309.11</v>
+      </c>
+      <c r="D25" s="77">
+        <f>C25/(1+(J25/100))</f>
+        <v>268.7913043478261</v>
+      </c>
+      <c r="E25" s="77">
+        <f>D25*21</f>
+        <v>5644.6173913043476</v>
+      </c>
+      <c r="F25" s="77">
+        <f>E25*12</f>
+        <v>67735.408695652179</v>
+      </c>
+      <c r="G25" s="80">
+        <f>D25/1.3/2</f>
+        <v>103.38127090301003</v>
+      </c>
+      <c r="H25" s="80">
+        <f>G25*21</f>
+        <v>2171.0066889632108</v>
+      </c>
+      <c r="I25" s="80">
+        <f>H25*12</f>
+        <v>26052.080267558529</v>
+      </c>
+      <c r="J25" s="73">
+        <v>15</v>
+      </c>
+      <c r="K25" s="74">
+        <f>I25*(1+(J25/100))</f>
+        <v>29959.892307692306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>1237</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="81">
+        <v>311.79000000000002</v>
+      </c>
+      <c r="D26" s="77">
+        <f>C26/(1+(J26/100))</f>
+        <v>257.67768595041326</v>
+      </c>
+      <c r="E26" s="77">
+        <f>D26*21</f>
+        <v>5411.2314049586785</v>
+      </c>
+      <c r="F26" s="77">
+        <f>E26*12</f>
+        <v>64934.776859504142</v>
+      </c>
+      <c r="G26" s="80">
+        <f>D26/1.3/2</f>
+        <v>99.106802288620486</v>
+      </c>
+      <c r="H26" s="80">
+        <f>G26*21</f>
+        <v>2081.2428480610301</v>
+      </c>
+      <c r="I26" s="80">
+        <f>H26*12</f>
+        <v>24974.91417673236</v>
+      </c>
+      <c r="J26" s="73">
+        <v>21</v>
+      </c>
+      <c r="K26" s="74">
+        <f>I26*(1+(J26/100))</f>
+        <v>30219.646153846155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J27" s="73"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J28" s="73"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>624</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="6">
+        <v>209.34</v>
+      </c>
+      <c r="D29" s="77">
+        <f t="shared" ref="D29:D30" si="0">C29/(1+(J29/100))</f>
+        <v>174.45000000000002</v>
+      </c>
+      <c r="E29" s="77">
+        <f t="shared" ref="E29:E30" si="1">D29*21</f>
+        <v>3663.4500000000003</v>
+      </c>
+      <c r="F29" s="77">
+        <f t="shared" ref="F29:F30" si="2">E29*12</f>
+        <v>43961.4</v>
+      </c>
+      <c r="G29" s="80">
+        <f t="shared" ref="G29:G30" si="3">D29/1.3/2</f>
+        <v>67.096153846153854</v>
+      </c>
+      <c r="H29" s="80">
+        <f t="shared" ref="H29:H30" si="4">G29*21</f>
+        <v>1409.0192307692309</v>
+      </c>
+      <c r="I29" s="80">
+        <f t="shared" ref="I29:I30" si="5">H29*12</f>
+        <v>16908.230769230773</v>
+      </c>
+      <c r="J29" s="73">
+        <v>20</v>
+      </c>
+      <c r="K29" s="74">
+        <f t="shared" ref="K29:K30" si="6">I29*(1+(J29/100))</f>
+        <v>20289.876923076929</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>1265</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" s="6">
+        <v>224.61</v>
+      </c>
+      <c r="D30" s="77">
+        <f t="shared" si="0"/>
+        <v>191.97435897435901</v>
+      </c>
+      <c r="E30" s="77">
+        <f t="shared" si="1"/>
+        <v>4031.461538461539</v>
+      </c>
+      <c r="F30" s="77">
+        <f t="shared" si="2"/>
+        <v>48377.538461538468</v>
+      </c>
+      <c r="G30" s="80">
+        <f t="shared" si="3"/>
+        <v>73.836291913215007</v>
+      </c>
+      <c r="H30" s="80">
+        <f t="shared" si="4"/>
+        <v>1550.5621301775152</v>
+      </c>
+      <c r="I30" s="80">
+        <f t="shared" si="5"/>
+        <v>18606.745562130181</v>
+      </c>
+      <c r="J30" s="73">
+        <v>17</v>
+      </c>
+      <c r="K30" s="74">
+        <f t="shared" si="6"/>
+        <v>21769.892307692309</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E33" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="72" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="72" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="C19:F20"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J21:K21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA0236E-5373-418A-9877-4E571B657A0C}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2993,31 +3383,31 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="42">
         <v>1366</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="56" t="s">
-        <v>175</v>
-      </c>
-      <c r="K2" s="56" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" s="46" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="4"/>
@@ -3031,113 +3421,113 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="C3" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="K3" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="66" t="s">
+    </row>
+    <row r="4" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="65" t="s">
-        <v>176</v>
-      </c>
-      <c r="K3" s="65" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="42">
+        <v>1366</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="62">
+        <v>95</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="60"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="K5" s="39"/>
+    </row>
+    <row r="6" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="51" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="52">
-        <v>1366</v>
-      </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="56" t="s">
-        <v>177</v>
-      </c>
-      <c r="K4" s="56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>166</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="72">
-        <v>95</v>
-      </c>
-      <c r="G5" s="70" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="K5" s="49"/>
-    </row>
-    <row r="6" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>